<commit_message>
Alg - Session 1 pdf
</commit_message>
<xml_diff>
--- a/Algoritmia/tables/lab1/tableDiagonal.xlsx
+++ b/Algoritmia/tables/lab1/tableDiagonal.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uo244965\Downloads\University\Algoritmia\tables\lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carla\Documents\Git\University\Algoritmia\tables\lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,32 +24,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>n</t>
   </si>
   <si>
-    <t>fillIn(t) (ms)</t>
+    <t>fillIn (micros)</t>
   </si>
   <si>
-    <t>sum1Diagonal(t) (ms)</t>
+    <t>sum1Diagonal (micros)</t>
   </si>
   <si>
-    <t>sum2Diagonal(t) (ms)</t>
+    <t>sum2Diagonal (micros)</t>
+  </si>
+  <si>
+    <t>theoretical</t>
+  </si>
+  <si>
+    <t>fillIn (theor)</t>
+  </si>
+  <si>
+    <t>sum1Diagonal (theor)</t>
+  </si>
+  <si>
+    <t>sum2Diagonal (theor)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="165" formatCode="0.000000"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -63,7 +78,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -71,16 +86,65 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -89,8 +153,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -112,7 +191,597 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fillIn (micros)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3072</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6144</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.46600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7589999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.9059999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>111.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>442.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2050</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7220</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>113660</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>457000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1825000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sum1Diagonal (micros)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3072</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6144</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$3:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>7.9469999999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2199999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.6500000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.40110000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77.739999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1111</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4429</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sum2Diagonal (micros)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3072</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6144</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$3:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2.1570000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5589999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6299999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8199999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1464</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.54910000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.61</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.8090000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="747809312"/>
+        <c:axId val="747818560"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="747809312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="747818560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="747818560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="747809312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -143,7 +812,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="es-ES"/>
               <a:t>fillIn</a:t>
             </a:r>
           </a:p>
@@ -175,7 +844,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -186,8 +855,149 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fillIn (micros)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3072</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6144</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.46600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7589999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.9059999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>111.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>442.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2050</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7220</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>113660</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>457000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1825000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fillIn (theor)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -214,7 +1024,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$14</c:f>
+              <c:f>Sheet1!$C$19:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -259,45 +1069,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$14</c:f>
+              <c:f>Sheet1!$D$19:$D$30</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>2.6499999999999999E-4</c:v>
+                  <c:v>0.14799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.4899999999999999E-4</c:v>
+                  <c:v>0.59199999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2620000000000001E-3</c:v>
+                  <c:v>2.3679999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2777E-2</c:v>
+                  <c:v>9.4719999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.2099999999999999E-2</c:v>
+                  <c:v>37.887999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.187</c:v>
+                  <c:v>151.55199999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.749</c:v>
+                  <c:v>606.20799999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.9489999999999998</c:v>
+                  <c:v>2424.8319999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.954000000000001</c:v>
+                  <c:v>9699.3279999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43.7</c:v>
+                  <c:v>38797.311999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>191.9</c:v>
+                  <c:v>155189.24799999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>773.8</c:v>
+                  <c:v>620756.99199999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -312,11 +1122,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="157343048"/>
-        <c:axId val="157770432"/>
+        <c:axId val="836292512"/>
+        <c:axId val="836295232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="157343048"/>
+        <c:axId val="836292512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -370,15 +1180,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157770432"/>
+        <c:crossAx val="836295232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="157770432"/>
+        <c:axId val="836295232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,7 +1208,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -432,10 +1242,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="157343048"/>
+        <c:crossAx val="836292512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -447,6 +1257,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -473,7 +1315,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -484,10 +1326,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -518,7 +1360,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="es-ES"/>
               <a:t>sum1Diagonal</a:t>
             </a:r>
           </a:p>
@@ -550,7 +1392,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -561,8 +1403,149 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sum1Diagonal (micros)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3072</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6144</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$3:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>7.9469999999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2199999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.6500000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.40110000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77.739999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1111</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4429</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sum1Diagonal (theor)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -589,7 +1572,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$14</c:f>
+              <c:f>Sheet1!$C$19:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -634,45 +1617,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$14</c:f>
+              <c:f>Sheet1!$E$19:$E$30</c:f>
               <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>6.2000000000000003E-5</c:v>
+                  <c:v>7.9469999999999992E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3E-5</c:v>
+                  <c:v>3.1787999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.03E-4</c:v>
+                  <c:v>0.12715199999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.6400000000000003E-4</c:v>
+                  <c:v>0.50860799999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0739999999999999E-3</c:v>
+                  <c:v>2.0344319999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2652999999999999E-2</c:v>
+                  <c:v>8.1377279999999992</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.3700000000000003E-2</c:v>
+                  <c:v>32.550911999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.67410000000000003</c:v>
+                  <c:v>130.20364799999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.67410000000000003</c:v>
+                  <c:v>520.81459199999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.373</c:v>
+                  <c:v>2083.2583679999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.5529999999999999</c:v>
+                  <c:v>8333.0334719999992</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22.31</c:v>
+                  <c:v>33332.133887999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -687,11 +1670,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="286385168"/>
-        <c:axId val="205881136"/>
+        <c:axId val="786727792"/>
+        <c:axId val="786718544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="286385168"/>
+        <c:axId val="786727792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -745,333 +1728,20 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="205881136"/>
+        <c:crossAx val="786718544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="205881136"/>
+        <c:axId val="786718544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="286385168"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>sum2Diagonal</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>192</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>384</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>768</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1536</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3072</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6144</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$3:$E$14</c:f>
-              <c:numCache>
-                <c:formatCode>0.000000</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>1.0900000000000001E-5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.3999999999999998E-6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.4E-5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.8099999999999999E-5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.6199999999999997E-5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1E-4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.2699999999999998E-4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.513E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.8539999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.8910000000000005E-3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.2417000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.1216</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="286971384"/>
-        <c:axId val="286970992"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="286971384"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1120,72 +1790,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="286970992"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="286970992"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="286971384"/>
+        <c:crossAx val="786727792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1197,6 +1805,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1223,7 +1863,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2906,20 +3546,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="6" name="Gráfico 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2936,20 +3576,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>585107</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1323975</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2966,20 +3606,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>186417</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>72117</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Gráfico 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2998,7 +3638,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3260,19 +3900,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3280,270 +3923,280 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="4">
+      <c r="B3" s="3"/>
+      <c r="C3" s="8">
         <v>3</v>
       </c>
-      <c r="C3" s="5">
-        <f>265/1000000</f>
-        <v>2.6499999999999999E-4</v>
-      </c>
-      <c r="D3" s="5">
-        <f>62/1000000</f>
-        <v>6.2000000000000003E-5</v>
-      </c>
-      <c r="E3" s="5">
-        <f>109/10000000</f>
-        <v>1.0900000000000001E-5</v>
-      </c>
-      <c r="F3" s="1"/>
+      <c r="D3" s="9">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="E3" s="9">
+        <f>7947/1000000</f>
+        <v>7.9469999999999992E-3</v>
+      </c>
+      <c r="F3" s="9">
+        <f>2157/1000000</f>
+        <v>2.1570000000000001E-3</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="4">
-        <f>B3*2</f>
+      <c r="B4" s="3"/>
+      <c r="C4" s="8">
         <v>6</v>
       </c>
-      <c r="C4" s="5">
-        <f>749/1000000</f>
-        <v>7.4899999999999999E-4</v>
-      </c>
-      <c r="D4" s="5">
-        <f>63/1000000</f>
-        <v>6.3E-5</v>
-      </c>
-      <c r="E4" s="5">
-        <f>94/10000000</f>
-        <v>9.3999999999999998E-6</v>
-      </c>
-      <c r="F4" s="1"/>
+      <c r="D4" s="9">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="E4" s="9">
+        <f>322/10000</f>
+        <v>3.2199999999999999E-2</v>
+      </c>
+      <c r="F4" s="9">
+        <v>4.5589999999999997E-3</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="4">
-        <f t="shared" ref="B5:B14" si="0">B4*2</f>
+      <c r="B5" s="3"/>
+      <c r="C5" s="8">
         <v>12</v>
       </c>
-      <c r="C5" s="5">
-        <f>3262/1000000</f>
-        <v>3.2620000000000001E-3</v>
-      </c>
-      <c r="D5" s="5">
-        <f>203/1000000</f>
-        <v>2.03E-4</v>
-      </c>
-      <c r="E5" s="5">
-        <f>140/10000000</f>
-        <v>1.4E-5</v>
-      </c>
-      <c r="F5" s="1"/>
+      <c r="D5" s="9">
+        <v>1.7589999999999999</v>
+      </c>
+      <c r="E5" s="9">
+        <v>9.6500000000000002E-2</v>
+      </c>
+      <c r="F5" s="9">
+        <f>83/10000</f>
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="4">
-        <f t="shared" si="0"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="8">
         <v>24</v>
       </c>
-      <c r="C6" s="5">
-        <f>12777/1000000</f>
-        <v>1.2777E-2</v>
-      </c>
-      <c r="D6" s="5">
-        <f>764/1000000</f>
-        <v>7.6400000000000003E-4</v>
-      </c>
-      <c r="E6" s="5">
-        <f>281/10000000</f>
-        <v>2.8099999999999999E-5</v>
-      </c>
-      <c r="F6" s="1"/>
+      <c r="D6" s="9">
+        <v>6.9059999999999997</v>
+      </c>
+      <c r="E6" s="9">
+        <f>4011/10000</f>
+        <v>0.40110000000000001</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1.6299999999999999E-2</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="4">
-        <f t="shared" si="0"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="8">
         <v>48</v>
       </c>
-      <c r="C7" s="5">
-        <f>421/10000</f>
-        <v>4.2099999999999999E-2</v>
-      </c>
-      <c r="D7" s="5">
-        <f>3074/1000000</f>
-        <v>3.0739999999999999E-3</v>
-      </c>
-      <c r="E7" s="5">
-        <f>562/10000000</f>
-        <v>5.6199999999999997E-5</v>
-      </c>
-      <c r="F7" s="1"/>
+      <c r="D7" s="9">
+        <v>27.4</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1.88</v>
+      </c>
+      <c r="F7" s="9">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="4">
-        <f t="shared" si="0"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="8">
         <v>96</v>
       </c>
-      <c r="C8" s="5">
-        <f>187/1000</f>
-        <v>0.187</v>
-      </c>
-      <c r="D8" s="5">
-        <f>12653/1000000</f>
-        <v>1.2652999999999999E-2</v>
-      </c>
-      <c r="E8" s="5">
-        <f>110/1000000</f>
-        <v>1.1E-4</v>
-      </c>
-      <c r="F8" s="1"/>
+      <c r="D8" s="9">
+        <v>111.3</v>
+      </c>
+      <c r="E8" s="9">
+        <v>6.26</v>
+      </c>
+      <c r="F8" s="9">
+        <v>6.8199999999999997E-2</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="4">
-        <f t="shared" si="0"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="8">
         <v>192</v>
       </c>
-      <c r="C9" s="5">
-        <f>749/1000</f>
-        <v>0.749</v>
-      </c>
-      <c r="D9" s="5">
-        <f>437/10000</f>
-        <v>4.3700000000000003E-2</v>
-      </c>
-      <c r="E9" s="5">
-        <f>327/1000000</f>
-        <v>3.2699999999999998E-4</v>
-      </c>
-      <c r="F9" s="1"/>
+      <c r="D9" s="9">
+        <v>442.6</v>
+      </c>
+      <c r="E9" s="9">
+        <v>21.54</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0.1464</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="4">
-        <f t="shared" si="0"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="8">
         <v>384</v>
       </c>
-      <c r="C10" s="5">
-        <f>2949/1000</f>
-        <v>2.9489999999999998</v>
-      </c>
-      <c r="D10" s="5">
-        <f>6741/10000</f>
-        <v>0.67410000000000003</v>
-      </c>
-      <c r="E10" s="5">
-        <f>1513/1000000</f>
-        <v>1.513E-3</v>
-      </c>
-      <c r="F10" s="1"/>
+      <c r="D10" s="9">
+        <v>2050</v>
+      </c>
+      <c r="E10" s="9">
+        <v>77.739999999999995</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.54910000000000003</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="4">
-        <f t="shared" si="0"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="8">
         <v>768</v>
       </c>
-      <c r="C11" s="5">
-        <f>11954/1000</f>
-        <v>11.954000000000001</v>
-      </c>
-      <c r="D11" s="5">
-        <f>6741/10000</f>
-        <v>0.67410000000000003</v>
-      </c>
-      <c r="E11" s="5">
-        <f>3854/1000000</f>
-        <v>3.8539999999999998E-3</v>
-      </c>
-      <c r="F11" s="1"/>
+      <c r="D11" s="9">
+        <v>7220</v>
+      </c>
+      <c r="E11" s="9">
+        <v>288</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="4">
-        <f t="shared" si="0"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="8">
         <v>1536</v>
       </c>
-      <c r="C12" s="5">
-        <f>437/10</f>
-        <v>43.7</v>
-      </c>
-      <c r="D12" s="5">
-        <f>1373/1000</f>
-        <v>1.373</v>
-      </c>
-      <c r="E12" s="5">
-        <f>9891/1000000</f>
-        <v>9.8910000000000005E-3</v>
-      </c>
-      <c r="F12" s="1"/>
+      <c r="D12" s="9">
+        <v>113660</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1111</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1.61</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="4">
-        <f t="shared" si="0"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="8">
         <v>3072</v>
       </c>
-      <c r="C13" s="5">
-        <f>1919/10</f>
-        <v>191.9</v>
-      </c>
-      <c r="D13" s="5">
-        <f>5553/1000</f>
-        <v>5.5529999999999999</v>
-      </c>
-      <c r="E13" s="5">
-        <f>32417/1000000</f>
-        <v>3.2417000000000001E-2</v>
-      </c>
-      <c r="F13" s="1"/>
+      <c r="D13" s="9">
+        <v>457000</v>
+      </c>
+      <c r="E13" s="9">
+        <v>4429</v>
+      </c>
+      <c r="F13" s="9">
+        <v>4.8090000000000002</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="4">
-        <f t="shared" si="0"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="8">
         <v>6144</v>
       </c>
-      <c r="C14" s="5">
-        <f>7738/10</f>
-        <v>773.8</v>
-      </c>
-      <c r="D14" s="5">
-        <f>2231/100</f>
-        <v>22.31</v>
-      </c>
-      <c r="E14" s="5">
-        <f>1216/10000</f>
-        <v>0.1216</v>
-      </c>
-      <c r="F14" s="1"/>
+      <c r="D14" s="9">
+        <v>1825000</v>
+      </c>
+      <c r="E14" s="9">
+        <v>17800</v>
+      </c>
+      <c r="F14" s="9">
+        <v>12.2</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -3551,82 +4204,250 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="C18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="C19" s="8">
+        <v>3</v>
+      </c>
+      <c r="D19" s="9">
+        <f>D3</f>
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="E19" s="9">
+        <f>E3</f>
+        <v>7.9469999999999992E-3</v>
+      </c>
+      <c r="F19" s="9">
+        <f>F3</f>
+        <v>2.1570000000000001E-3</v>
+      </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="C20" s="8">
+        <v>6</v>
+      </c>
+      <c r="D20" s="9">
+        <f>(POWER(C20,2)/POWER($C$19,2))*$D$19</f>
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="E20" s="9">
+        <f>(POWER(C20,2)/POWER($C$19,2))*$E$19</f>
+        <v>3.1787999999999997E-2</v>
+      </c>
+      <c r="F20" s="9">
+        <f>(C20/$C$19)*$F$19</f>
+        <v>4.3140000000000001E-3</v>
+      </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="8">
+        <v>12</v>
+      </c>
+      <c r="D21" s="9">
+        <f t="shared" ref="D21:D30" si="0">(POWER(C21,2)/POWER($C$19,2))*$D$19</f>
+        <v>2.3679999999999999</v>
+      </c>
+      <c r="E21" s="9">
+        <f t="shared" ref="E21:E30" si="1">(POWER(C21,2)/POWER($C$19,2))*$E$19</f>
+        <v>0.12715199999999999</v>
+      </c>
+      <c r="F21" s="9">
+        <f t="shared" ref="F21:F30" si="2">(C21/$C$19)*$F$19</f>
+        <v>8.6280000000000003E-3</v>
+      </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="8">
+        <v>24</v>
+      </c>
+      <c r="D22" s="9">
+        <f t="shared" si="0"/>
+        <v>9.4719999999999995</v>
+      </c>
+      <c r="E22" s="9">
+        <f t="shared" si="1"/>
+        <v>0.50860799999999995</v>
+      </c>
+      <c r="F22" s="9">
+        <f t="shared" si="2"/>
+        <v>1.7256000000000001E-2</v>
+      </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="8">
+        <v>48</v>
+      </c>
+      <c r="D23" s="9">
+        <f t="shared" si="0"/>
+        <v>37.887999999999998</v>
+      </c>
+      <c r="E23" s="9">
+        <f t="shared" si="1"/>
+        <v>2.0344319999999998</v>
+      </c>
+      <c r="F23" s="9">
+        <f t="shared" si="2"/>
+        <v>3.4512000000000001E-2</v>
+      </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="1"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="8">
+        <v>96</v>
+      </c>
+      <c r="D24" s="9">
+        <f t="shared" si="0"/>
+        <v>151.55199999999999</v>
+      </c>
+      <c r="E24" s="9">
+        <f t="shared" si="1"/>
+        <v>8.1377279999999992</v>
+      </c>
+      <c r="F24" s="9">
+        <f t="shared" si="2"/>
+        <v>6.9024000000000002E-2</v>
+      </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="1"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="8">
+        <v>192</v>
+      </c>
+      <c r="D25" s="9">
+        <f t="shared" si="0"/>
+        <v>606.20799999999997</v>
+      </c>
+      <c r="E25" s="9">
+        <f t="shared" si="1"/>
+        <v>32.550911999999997</v>
+      </c>
+      <c r="F25" s="9">
+        <f t="shared" si="2"/>
+        <v>0.138048</v>
+      </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+    <row r="26" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="2"/>
+      <c r="C26" s="8">
+        <v>384</v>
+      </c>
+      <c r="D26" s="9">
+        <f t="shared" si="0"/>
+        <v>2424.8319999999999</v>
+      </c>
+      <c r="E26" s="9">
+        <f t="shared" si="1"/>
+        <v>130.20364799999999</v>
+      </c>
+      <c r="F26" s="9">
+        <f t="shared" si="2"/>
+        <v>0.27609600000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="8">
+        <v>768</v>
+      </c>
+      <c r="D27" s="9">
+        <f t="shared" si="0"/>
+        <v>9699.3279999999995</v>
+      </c>
+      <c r="E27" s="9">
+        <f t="shared" si="1"/>
+        <v>520.81459199999995</v>
+      </c>
+      <c r="F27" s="9">
+        <f t="shared" si="2"/>
+        <v>0.55219200000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="8">
+        <v>1536</v>
+      </c>
+      <c r="D28" s="9">
+        <f t="shared" si="0"/>
+        <v>38797.311999999998</v>
+      </c>
+      <c r="E28" s="9">
+        <f t="shared" si="1"/>
+        <v>2083.2583679999998</v>
+      </c>
+      <c r="F28" s="9">
+        <f t="shared" si="2"/>
+        <v>1.104384</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="8">
+        <v>3072</v>
+      </c>
+      <c r="D29" s="9">
+        <f t="shared" si="0"/>
+        <v>155189.24799999999</v>
+      </c>
+      <c r="E29" s="9">
+        <f t="shared" si="1"/>
+        <v>8333.0334719999992</v>
+      </c>
+      <c r="F29" s="9">
+        <f t="shared" si="2"/>
+        <v>2.2087680000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="8">
+        <v>6144</v>
+      </c>
+      <c r="D30" s="9">
+        <f t="shared" si="0"/>
+        <v>620756.99199999997</v>
+      </c>
+      <c r="E30" s="9">
+        <f t="shared" si="1"/>
+        <v>33332.133887999997</v>
+      </c>
+      <c r="F30" s="9">
+        <f t="shared" si="2"/>
+        <v>4.4175360000000001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>